<commit_message>
- autodoc site update
</commit_message>
<xml_diff>
--- a/test_product_detailed.xlsx
+++ b/test_product_detailed.xlsx
@@ -535,7 +535,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.autodoc.parts/ridex/8095160</t>
+          <t>https://www.autodoc.co.uk/ridex/8095160</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -546,17 +546,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7,59 €</t>
+          <t>£7. 59</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-48%</t>
+          <t>-42%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>